<commit_message>
update signature chapter to remove nanopore and add adult AML
</commit_message>
<xml_diff>
--- a/data/ewas_top_cpgs_os_aml_signature.xlsx
+++ b/data/ewas_top_cpgs_os_aml_signature.xlsx
@@ -748,7 +748,7 @@
     <t>RSPH14</t>
   </si>
   <si>
-    <t>TAF15;RASL10B</t>
+    <t>RASL10B;TAF15</t>
   </si>
   <si>
     <t>RP11-68I18.10</t>
@@ -799,7 +799,7 @@
     <t>EDARADD</t>
   </si>
   <si>
-    <t>FIP1L1;LNX1;LNX1-AS1</t>
+    <t>LNX1-AS1;FIP1L1;LNX1</t>
   </si>
   <si>
     <t>GPT2</t>
@@ -856,7 +856,7 @@
     <t>HK2</t>
   </si>
   <si>
-    <t>FXR2;SHBG</t>
+    <t>SHBG;FXR2</t>
   </si>
   <si>
     <t>LINC01140;RP5-1052I5.2</t>
@@ -874,10 +874,10 @@
     <t>RP11-99J16__A.2;CAPN9</t>
   </si>
   <si>
-    <t>FLCN;MPRIP;RP11-45M22.4</t>
-  </si>
-  <si>
-    <t>RP11-449P15.1;C7orf50;GPR146</t>
+    <t>MPRIP;RP11-45M22.4;FLCN</t>
+  </si>
+  <si>
+    <t>GPR146;RP11-449P15.1;C7orf50</t>
   </si>
   <si>
     <t>SUMO3</t>
@@ -949,7 +949,7 @@
     <t>SPEF1</t>
   </si>
   <si>
-    <t>RP11-374P20.4;BRD3</t>
+    <t>BRD3;RP11-374P20.4</t>
   </si>
   <si>
     <t>LAP3</t>
@@ -970,7 +970,7 @@
     <t>AGAP2;TSPAN31</t>
   </si>
   <si>
-    <t>RP11-77H9.2;PMM2;RP11-152P23.2</t>
+    <t>PMM2;RP11-152P23.2;RP11-77H9.2</t>
   </si>
   <si>
     <t>YWHAG</t>
@@ -991,7 +991,7 @@
     <t>SIGLEC10</t>
   </si>
   <si>
-    <t>SLC35E2B;MMP23B;CDK11B</t>
+    <t>CDK11B;SLC35E2B;MMP23B</t>
   </si>
   <si>
     <t>CAMKMT;PREPL</t>
@@ -1048,7 +1048,7 @@
     <t>ST18</t>
   </si>
   <si>
-    <t>AC114730.3;NEU4</t>
+    <t>NEU4;AC114730.3</t>
   </si>
   <si>
     <t>KRAS</t>
@@ -1135,7 +1135,7 @@
     <t>HDAC11</t>
   </si>
   <si>
-    <t>KLK6;CTB-147C22.9</t>
+    <t>CTB-147C22.9;KLK6</t>
   </si>
   <si>
     <t>ABHD8;MRPL34</t>
@@ -1165,7 +1165,7 @@
     <t>OBSCN</t>
   </si>
   <si>
-    <t>FBLN7;RP11-399B17.1</t>
+    <t>RP11-399B17.1;FBLN7</t>
   </si>
   <si>
     <t>RP5-902P8.12</t>
@@ -1213,7 +1213,7 @@
     <t>unitary_pseudogene;processed_transcript</t>
   </si>
   <si>
-    <t>antisense;protein_coding</t>
+    <t>protein_coding;antisense</t>
   </si>
   <si>
     <t>protein_coding;sense_intronic</t>
@@ -1231,10 +1231,10 @@
     <t>lincRNA;protein_coding</t>
   </si>
   <si>
-    <t>protein_coding;sense_overlapping</t>
-  </si>
-  <si>
-    <t>TEC;protein_coding</t>
+    <t>sense_overlapping;protein_coding</t>
+  </si>
+  <si>
+    <t>protein_coding;TEC</t>
   </si>
   <si>
     <t>S_Shore</t>

</xml_diff>